<commit_message>
Fix my varibles and CodeBook description
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501375C2-2F3E-4F2D-815D-069E24E212C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239DC5C7-26F6-4E9E-A7C2-B4B707F8C22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22230" yWindow="-120" windowWidth="19755" windowHeight="11985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Height</t>
   </si>
@@ -90,6 +90,24 @@
   </si>
   <si>
     <t>grey</t>
+  </si>
+  <si>
+    <t>sixty</t>
+  </si>
+  <si>
+    <t>Hair color</t>
+  </si>
+  <si>
+    <t>Shoe Size in MEN</t>
+  </si>
+  <si>
+    <t>Color of hair as of 2024/01</t>
+  </si>
+  <si>
+    <t>0-24</t>
+  </si>
+  <si>
+    <t>Any Color</t>
   </si>
 </sst>
 </file>
@@ -418,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,8 +494,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>60</v>
+      <c r="A4" t="s">
+        <v>23</v>
       </c>
       <c r="B4">
         <v>60</v>
@@ -597,6 +615,9 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>145</v>
+      </c>
+      <c r="B11">
+        <v>7000</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -680,10 +701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,6 +758,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Assignment 3: Coding Basics updates
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239DC5C7-26F6-4E9E-A7C2-B4B707F8C22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B036732-DD7A-4D58-9E2F-F3421B6DCA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22230" yWindow="-120" windowWidth="19755" windowHeight="11985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18615" yWindow="1290" windowWidth="17400" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Height</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>grey</t>
-  </si>
-  <si>
-    <t>sixty</t>
   </si>
   <si>
     <t>Hair color</t>
@@ -436,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,8 +491,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>23</v>
+      <c r="A4">
+        <v>60</v>
       </c>
       <c r="B4">
         <v>60</v>
@@ -617,7 +614,7 @@
         <v>145</v>
       </c>
       <c r="B11">
-        <v>7000</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -703,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -763,21 +760,21 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>